<commit_message>
Adding Automation Exercise Logout
</commit_message>
<xml_diff>
--- a/Creating User Accounts/Data/Output/Result.xlsx
+++ b/Creating User Accounts/Data/Output/Result.xlsx
@@ -52,7 +52,7 @@
     <x:t>Password</x:t>
   </x:si>
   <x:si>
-    <x:t>442</x:t>
+    <x:t>183</x:t>
   </x:si>
   <x:si>
     <x:t>Male</x:t>
@@ -61,100 +61,100 @@
     <x:t>United States</x:t>
   </x:si>
   <x:si>
-    <x:t>David</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Byrd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1948-01-30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1579 B StreetSaint Paul, MN 55104</x:t>
-  </x:si>
-  <x:si>
-    <x:t>651-532-9175</x:t>
+    <x:t>Shane</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Paz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1972-06-03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>471 Waterview LanePena Blanca, NM 87041</x:t>
+  </x:si>
+  <x:si>
+    <x:t>505-465-5925</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>Matrix Interior Design</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Plating and coating machine setter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>igacheP5chaeW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>508</x:t>
+    <x:t>Simply Appraisals</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Orthotics technician</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sieKa5uDie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>174</x:t>
   </x:si>
   <x:si>
     <x:t>Female</x:t>
   </x:si>
   <x:si>
-    <x:t>Australiaa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tammy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hughes</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1963-09-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8 Gregory WayBANKSIADALE WA 6213</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(08) 9438 4198</x:t>
+    <x:t>Australia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sylvia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Allen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2003-05-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54 Wallis StreetROSE BAY NORTH NSW 2030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(02) 9579 8213</x:t>
   </x:si>
   <x:si>
     <x:t>61</x:t>
   </x:si>
   <x:si>
-    <x:t>Rogersound Labs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fire investigator</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nasha9yie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>603</x:t>
-  </x:si>
-  <x:si>
-    <x:t>New Zealand</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bertha</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thomas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1950-08-26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>170 Stanley DriveKoutuRotorua 3010</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(020) 2511-915</x:t>
+    <x:t>Cut Rite</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Webmaster</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ahxeiJoo6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>155</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New Zealands</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Carol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Schmidt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1960-02-02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 Hautana StreetBoulcottLower Hutt 5010</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(028) 6342-658</x:t>
   </x:si>
   <x:si>
     <x:t>64</x:t>
   </x:si>
   <x:si>
-    <x:t>Miller &amp; Rhoads</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Aircraft and avionics equipment mechanic</x:t>
-  </x:si>
-  <x:si>
-    <x:t>phael2Ke8W</x:t>
+    <x:t>Incluesiv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Museum director</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aiNguLaiN9</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>